<commit_message>
Custom waste spreading by category and activity (part 8)
</commit_message>
<xml_diff>
--- a/waste_flow/extra_data_xls/waste_spreading.xlsx
+++ b/waste_flow/extra_data_xls/waste_spreading.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26120" yWindow="11840" windowWidth="24640" windowHeight="14160" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="17500" yWindow="6740" windowWidth="24640" windowHeight="14160" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="2" r:id="rId1"/>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1034,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
waste experts advised to change coefficients in waste_spreading.xlsx
</commit_message>
<xml_diff>
--- a/waste_flow/extra_data_xls/waste_spreading.xlsx
+++ b/waste_flow/extra_data_xls/waste_spreading.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sinclair/repos/sinclair/work/ispra_italy/repos/waste_flow/waste_flow/extra_data_xls/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\monitor4be\indicators\fromBiomassStudy\waste\waste_flow\waste_flow\extra_data_xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A618EE8-D5A9-4CEA-A1A0-E45B7E092D87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="13320" windowWidth="27380" windowHeight="15480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="12390" yWindow="615" windowWidth="15195" windowHeight="11385" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="2" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="C10-C12" sheetId="4" r:id="rId4"/>
     <sheet name="G-U_X_G4677" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -102,7 +103,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -162,6 +163,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -429,20 +433,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="138" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -471,7 +475,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -482,18 +486,18 @@
         <v>0.15049999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>8.0000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -504,18 +508,18 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="E5">
-        <v>0.54</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>8.0000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -523,7 +527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -534,7 +538,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -542,32 +546,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -578,20 +582,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="138" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -620,42 +624,42 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -666,7 +670,7 @@
         <v>0.15049999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -677,7 +681,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -688,7 +692,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -699,21 +703,21 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="C13">
+        <v>0.54</v>
+      </c>
+      <c r="E13">
         <v>0.4</v>
       </c>
-      <c r="E13">
-        <v>0.54</v>
-      </c>
       <c r="I13">
-        <v>5.1999999999999995E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>2.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -727,20 +731,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="138" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -769,7 +773,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -780,18 +784,18 @@
         <v>0.15049999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>8.0000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -802,18 +806,18 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="E5">
-        <v>0.54</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>8.0000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -824,7 +828,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -835,7 +839,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -843,32 +847,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -879,20 +883,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="138" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -921,7 +925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -932,18 +936,18 @@
         <v>0.15049999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>8.0000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -954,18 +958,18 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="E5">
-        <v>0.54</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>8.0000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -976,7 +980,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -987,7 +991,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -995,32 +999,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1031,20 +1035,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" zoomScalePageLayoutView="138" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -1073,7 +1077,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1084,18 +1088,18 @@
         <v>0.15049999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>8.0000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1106,18 +1110,18 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="E5">
-        <v>0.54</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>8.0000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1128,7 +1132,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1139,7 +1143,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1147,32 +1151,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
coefficients updated by waste experts
</commit_message>
<xml_diff>
--- a/waste_flow/extra_data_xls/waste_spreading.xlsx
+++ b/waste_flow/extra_data_xls/waste_spreading.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\monitor4be\indicators\fromBiomassStudy\waste\waste_flow\waste_flow\extra_data_xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A618EE8-D5A9-4CEA-A1A0-E45B7E092D87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20F2B54-06CD-44BF-A210-EEB2361534FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12390" yWindow="615" windowWidth="15195" windowHeight="11385" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13980" yWindow="570" windowWidth="15195" windowHeight="11385" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="2" r:id="rId1"/>
@@ -886,7 +886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="138" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="138" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1038,7 +1038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" zoomScalePageLayoutView="138" workbookViewId="0">
+    <sheetView zoomScale="87" zoomScaleNormal="87" zoomScalePageLayoutView="138" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated coefficients from waste experts
</commit_message>
<xml_diff>
--- a/waste_flow/extra_data_xls/waste_spreading.xlsx
+++ b/waste_flow/extra_data_xls/waste_spreading.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\monitor4be\indicators\fromBiomassStudy\waste\waste_flow\waste_flow\extra_data_xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20F2B54-06CD-44BF-A210-EEB2361534FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D79A61-CE86-429B-80F0-975D7726797F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13980" yWindow="570" windowWidth="15195" windowHeight="11385" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14790" yWindow="525" windowWidth="11985" windowHeight="14055" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="2" r:id="rId1"/>
@@ -19,10 +19,19 @@
     <sheet name="C10-C12" sheetId="4" r:id="rId4"/>
     <sheet name="G-U_X_G4677" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -436,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="138" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -491,10 +500,11 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="I3">
-        <v>2.3999999999999998E-3</v>
+        <f>0.014/3</f>
+        <v>4.6666666666666671E-3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -505,7 +515,7 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>7.4999999999999997E-3</v>
+        <v>4.4999999999999997E-3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -513,10 +523,11 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.54</v>
       </c>
       <c r="I5">
-        <v>2.3999999999999998E-3</v>
+        <f>0.014/3</f>
+        <v>4.6666666666666671E-3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -586,7 +597,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -678,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="I10">
-        <v>7.4999999999999997E-3</v>
+        <v>4.4999999999999997E-3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -714,7 +725,8 @@
         <v>0.4</v>
       </c>
       <c r="I13">
-        <v>2.3999999999999998E-3</v>
+        <f>0.014/3</f>
+        <v>4.6666666666666671E-3</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -735,7 +747,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -789,10 +801,11 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="I3">
-        <v>2.3999999999999998E-3</v>
+        <f>0.014/3</f>
+        <v>4.6666666666666671E-3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -803,7 +816,7 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>7.4999999999999997E-3</v>
+        <v>4.4999999999999997E-3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -811,10 +824,11 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.54</v>
       </c>
       <c r="I5">
-        <v>2.3999999999999998E-3</v>
+        <f>0.014/3</f>
+        <v>4.6666666666666671E-3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -886,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="138" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -941,10 +955,11 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="I3">
-        <v>2.3999999999999998E-3</v>
+        <f>0.014/3</f>
+        <v>4.6666666666666671E-3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -955,7 +970,7 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>7.4999999999999997E-3</v>
+        <v>4.4999999999999997E-3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -963,10 +978,11 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.54</v>
       </c>
       <c r="I5">
-        <v>2.3999999999999998E-3</v>
+        <f>0.014/3</f>
+        <v>4.6666666666666671E-3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1039,7 +1055,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScale="87" zoomScaleNormal="87" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1093,10 +1109,11 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="I3">
-        <v>2.3999999999999998E-3</v>
+        <f>0.014/3</f>
+        <v>4.6666666666666671E-3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1107,7 +1124,7 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>7.4999999999999997E-3</v>
+        <v>4.4999999999999997E-3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1115,10 +1132,11 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.54</v>
       </c>
       <c r="I5">
-        <v>2.3999999999999998E-3</v>
+        <f>0.014/3</f>
+        <v>4.6666666666666671E-3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>